<commit_message>
Added IDs to crime folder
</commit_message>
<xml_diff>
--- a/suspectDB2.xlsx
+++ b/suspectDB2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Suspect" sheetId="1" r:id="rId1"/>
@@ -568,9 +568,6 @@
     <t>Pornography/Obscene Material</t>
   </si>
   <si>
-    <t>Kindapping/Abduction</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -694,9 +691,6 @@
     <t>Human Trafficking, Involuntary Servitude</t>
   </si>
   <si>
-    <t>Indentity Theft</t>
-  </si>
-  <si>
     <t>Impersonation</t>
   </si>
   <si>
@@ -779,6 +773,12 @@
   </si>
   <si>
     <t>Wire Fraud</t>
+  </si>
+  <si>
+    <t>Identity Theft</t>
+  </si>
+  <si>
+    <t>Kidnapping/Abduction</t>
   </si>
 </sst>
 </file>
@@ -1128,28 +1128,28 @@
         <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>190</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>2</v>
@@ -1175,10 +1175,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D2" s="3">
         <v>1967</v>
@@ -1196,7 +1196,7 @@
         <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>9</v>
@@ -1222,10 +1222,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D3" s="3">
         <v>1967</v>
@@ -1241,7 +1241,7 @@
         <v>14</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>9</v>
@@ -1267,10 +1267,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D4" s="3">
         <v>1976</v>
@@ -1340,7 +1340,7 @@
         <v>123</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2217,8 +2217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2237,16 +2237,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2254,7 +2254,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2265,7 +2265,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -2276,7 +2276,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2308,7 +2308,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -2319,7 +2319,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2330,7 +2330,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2341,7 +2341,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -2352,7 +2352,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -2363,7 +2363,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2374,7 +2374,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -2385,7 +2385,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2396,7 +2396,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -2407,7 +2407,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2418,7 +2418,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -2429,7 +2429,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -2440,7 +2440,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2451,7 +2451,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -2462,7 +2462,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -2473,7 +2473,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2484,7 +2484,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2495,7 +2495,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2506,7 +2506,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2517,7 +2517,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2528,7 +2528,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -2539,7 +2539,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -2550,7 +2550,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>179</v>
+        <v>249</v>
       </c>
       <c r="C28" s="2">
         <v>16636</v>
@@ -2571,7 +2571,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -2582,7 +2582,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2593,7 +2593,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -2604,7 +2604,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2612,7 +2612,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -2644,7 +2644,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2655,7 +2655,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2666,7 +2666,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2677,7 +2677,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2685,7 +2685,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -2696,7 +2696,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -2707,7 +2707,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -2718,7 +2718,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2729,7 +2729,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2740,7 +2740,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2751,7 +2751,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2762,7 +2762,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2773,7 +2773,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2784,7 +2784,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -2795,7 +2795,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2806,7 +2806,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2817,7 +2817,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -2828,7 +2828,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2839,7 +2839,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2863,7 +2863,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>177</v>
@@ -2942,7 +2942,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>176</v>
@@ -2981,7 +2981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2998,16 +2998,16 @@
         <v>176</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>